<commit_message>
Updated the Test Plan for SwagLabs
Created additional test scenarios for the full web page functionalities.
</commit_message>
<xml_diff>
--- a/SwagLabsDocumentation/SwagLabs_DesignRequirements.xlsx
+++ b/SwagLabsDocumentation/SwagLabs_DesignRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Branimir\Documents\GitHub\RoxoftTask\RoxoftTask\SwagLabsDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DFF24A-684A-4CFC-BEAC-04AF6F24450F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E54CD-11C8-4BED-8CD7-0BA9C0D53838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Requirement mark</t>
   </si>
@@ -60,6 +60,9 @@
     <t>3.1.3</t>
   </si>
   <si>
+    <t>3.1.4</t>
+  </si>
+  <si>
     <t>3.2.1</t>
   </si>
   <si>
@@ -114,12 +117,6 @@
     <t>All Items element should return you to the homepage and show all the shopping inventory items on the homepage.</t>
   </si>
   <si>
-    <t>About element should take you to https://saucelabs.com/.</t>
-  </si>
-  <si>
-    <t>The Logout element should log you out from the home page and return you to the login page.</t>
-  </si>
-  <si>
     <t>Each inventory item element on the home page should have a picture, a title, the description of the item, the price and an "Add to Cart" button.</t>
   </si>
   <si>
@@ -151,6 +148,15 @@
   </si>
   <si>
     <t>The "Name (A to Z)" option, should filter the homepage options alphabetically, in ascending order.</t>
+  </si>
+  <si>
+    <t>About element should be clickable, and take you to https://saucelabs.com/.</t>
+  </si>
+  <si>
+    <t>The Logout element should be clickable, and log you out from the home page and return you to the login page.</t>
+  </si>
+  <si>
+    <t>The ResetAppState element should be clickable, and reset the app to its default state.</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,12 +224,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -416,14 +416,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -431,13 +428,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -452,29 +443,32 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,10 +764,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5"/>
@@ -790,8 +784,8 @@
       <c r="N1" s="4"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="5"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -806,10 +800,10 @@
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
@@ -826,11 +820,11 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>20</v>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -846,11 +840,11 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>21</v>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -866,11 +860,11 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>22</v>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -886,11 +880,11 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>27</v>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -906,10 +900,10 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="15">
         <v>2</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
@@ -926,11 +920,11 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="16">
         <v>2.1</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>23</v>
+      <c r="B9" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -946,11 +940,11 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="16">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>24</v>
+      <c r="B10" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -966,11 +960,11 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="16">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>25</v>
+      <c r="B11" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -986,11 +980,11 @@
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
+      <c r="A12" s="23">
         <v>2.4</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>26</v>
+      <c r="B12" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1006,11 +1000,11 @@
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="15">
         <v>3</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>33</v>
+      <c r="B13" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1026,10 +1020,10 @@
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="16">
         <v>3.1</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2"/>
@@ -1046,11 +1040,11 @@
       <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>28</v>
+      <c r="B15" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1066,11 +1060,11 @@
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>29</v>
+      <c r="B16" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1086,11 +1080,11 @@
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>30</v>
+      <c r="B17" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1106,11 +1100,11 @@
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <v>3.2</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>31</v>
+      <c r="A18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1126,11 +1120,11 @@
       <c r="N18" s="2"/>
     </row>
     <row r="19" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>35</v>
+      <c r="A19" s="16">
+        <v>3.2</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1146,11 +1140,11 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>36</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1166,31 +1160,31 @@
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
         <v>3.3</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>41</v>
+      <c r="B22" s="21" t="s">
+        <v>31</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1206,10 +1200,10 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="3"/>
@@ -1226,10 +1220,10 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="3"/>
@@ -1246,10 +1240,10 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="3"/>
@@ -1266,11 +1260,11 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>17</v>
+      <c r="B26" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1285,12 +1279,12 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:14" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>19</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1305,12 +1299,32 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="20">
+    <row r="28" spans="1:14" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
         <v>3.5</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>37</v>
+      <c r="B29" s="21" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>